<commit_message>
Updating my comments and fixing a few bugs
</commit_message>
<xml_diff>
--- a/Japallum_Apparel/DAL/Data_Dictonary.xlsx
+++ b/Japallum_Apparel/DAL/Data_Dictonary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monolith\Desktop\Projects\INFT-3050-web-programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monolith\Desktop\Projects\INFT-3050-web-programming\Japallum_Apparel\DAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83787620-F551-4086-8E2D-E8A064EF2846}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CACBAD0-8E73-4572-A202-ABBE90D7D56A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BCA443CA-9BD8-47A8-B013-DA655F05E55C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="86">
   <si>
     <t>Customer</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>Foreign Key References AdminID</t>
+  </si>
+  <si>
+    <t>customerActive</t>
+  </si>
+  <si>
+    <t>bit</t>
   </si>
 </sst>
 </file>
@@ -692,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423C33E5-2E8B-4D17-8720-2B38F06ABDF5}">
-  <dimension ref="B2:D76"/>
+  <dimension ref="B2:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,50 +803,50 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
@@ -849,466 +855,475 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D42" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>44</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D64" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D67" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D69" s="3"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D70" s="3"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="4" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" s="3"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="3"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D76" s="3"/>
+      <c r="D77" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Postage page and updates
</commit_message>
<xml_diff>
--- a/Japallum_Apparel/DAL/Data_Dictonary.xlsx
+++ b/Japallum_Apparel/DAL/Data_Dictonary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monolith\Desktop\Projects\INFT-3050-web-programming\Japallum_Apparel\DAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6376F5-1CF8-4780-B4FD-247DA0959D00}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E4785A-CDFD-4540-A602-0A35EBD3699C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BCA443CA-9BD8-47A8-B013-DA655F05E55C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
   <si>
     <t>Customer</t>
   </si>
@@ -683,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423C33E5-2E8B-4D17-8720-2B38F06ABDF5}">
-  <dimension ref="B2:D66"/>
+  <dimension ref="B2:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,6 +1224,15 @@
       </c>
       <c r="D66" s="3"/>
     </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>